<commit_message>
add: License in installer and fix not find icon in folder
</commit_message>
<xml_diff>
--- a/src/backend/pyengineer/templates/excel_template.xlsx
+++ b/src/backend/pyengineer/templates/excel_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\PyEngineer\src\examples\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\PyEngineerView\src\backend\src\examples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D57FD4-0E5C-4A07-AF95-09B45FFA3D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D4F324-F164-42D9-8837-B92EC4AC1BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="7" xr2:uid="{17B9D78E-9B11-469E-9BF6-00D2F9C8B7DE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="86">
   <si>
     <t>E</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>FDB4</t>
+  </si>
+  <si>
+    <t>FDB5</t>
+  </si>
+  <si>
+    <t>FDB6</t>
   </si>
 </sst>
 </file>
@@ -353,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -365,6 +371,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1899,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74033608-E1CC-4E7B-B66A-375D48222978}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1913,8 +1922,7 @@
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="8.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2084,53 +2092,55 @@
         <v>81</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1000</v>
-      </c>
-      <c r="G4" s="3">
-        <v>-3000</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>-1000</v>
+      </c>
+      <c r="M4" s="5">
+        <v>2000</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -2140,48 +2150,154 @@
         <v>72</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>-3000</v>
       </c>
       <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
         <v>-2000</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I6" s="3">
         <v>-2000</v>
       </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3">
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="M7" s="3">
+        <v>2000</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2239,16 +2355,16 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Célula Bloqueada" error="Não modifique os títulos!_x000a_Isso causará erro!" promptTitle="Momento em Z Final (N*m)" prompt="Momento na direção do eixo &quot;z&quot; no final da barra." sqref="Q1" xr:uid="{B7FC6F06-3F68-48D8-99B5-C44B3E6CA6D4}">
       <formula1>"bloqueada"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2:A5" xr:uid="{82EC8606-F12C-4DFE-AD5B-35F10C607376}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um texto._x000a_- Certifíque-se de que não seja um número." sqref="A2:A7" xr:uid="{82EC8606-F12C-4DFE-AD5B-35F10C607376}">
       <formula1>ISTEXT(A2)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número&gt;= 0._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="D2:D5" xr:uid="{C949EF88-D82D-4A0B-AD21-9964D0ECF74A}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número&gt;= 0._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="D2:D7" xr:uid="{C949EF88-D82D-4A0B-AD21-9964D0ECF74A}">
       <formula1>AND(D2&gt;=0,ISNUMBER(D2))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número &gt; 0._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="E2:E5" xr:uid="{02820B3E-1F21-493D-AB01-9CDD983C27DD}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número &gt; 0._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="E2:E7" xr:uid="{02820B3E-1F21-493D-AB01-9CDD983C27DD}">
       <formula1>AND(E2&gt;0,ISNUMBER(E2))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="F2:Q5" xr:uid="{90240017-4CFE-4872-BBD0-B8570585AC9A}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Insira um número._x000a_- Deve ser um número do excel e não um texto._x000a_- Cuidado para não usar &quot;.&quot; em vez de &quot;,&quot; ou vice versa de acordo com sua configuração." sqref="F2:Q7" xr:uid="{90240017-4CFE-4872-BBD0-B8570585AC9A}">
       <formula1>ISNUMBER(F2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -2260,13 +2376,13 @@
           <x14:formula1>
             <xm:f>Data!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C5</xm:sqref>
+          <xm:sqref>C2:C7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Barra Inexistente" error="Insira uma barra cadastrada na aba &quot;Bars&quot;." xr:uid="{18DD2507-D3D0-4E5B-A5ED-932D11D7A9F9}">
           <x14:formula1>
             <xm:f>OFFSET(Bars!$A$2,0,0,COUNTA(Bars!$A:$A)-1,1)</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B5</xm:sqref>
+          <xm:sqref>B2:B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>